<commit_message>
spa 24h results added
</commit_message>
<xml_diff>
--- a/Results_stats.xlsx
+++ b/Results_stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/46a44a3920e591ab/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\GitHub\KrosseKrabbeRacing.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E5ED5DD-5E60-42D7-89F1-14D7117FC17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0249F67-0C9C-4AEA-A8C3-F49B9DA45438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3450" yWindow="2760" windowWidth="21600" windowHeight="11295" xr2:uid="{09592AC9-B2E9-4EDE-80C7-AD726B4E7CCE}"/>
+    <workbookView xWindow="-23025" yWindow="2550" windowWidth="13095" windowHeight="7800" xr2:uid="{09592AC9-B2E9-4EDE-80C7-AD726B4E7CCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Laps</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Nürnburgring Combined</t>
+  </si>
+  <si>
+    <t>Spa Endurance</t>
   </si>
 </sst>
 </file>
@@ -431,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCCAFD40-2A12-4AC5-AD04-8D79316F0C6D}">
-  <dimension ref="B1:H5"/>
+  <dimension ref="B1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,19 +448,19 @@
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <f>SUM(B4:B1000)</f>
-        <v>51</v>
+        <v>604</v>
       </c>
       <c r="C1" s="1">
         <f t="shared" ref="C1:E1" si="0">SUM(C4:C1000)</f>
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>171</v>
       </c>
       <c r="E1" s="1">
         <f t="shared" si="0"/>
-        <v>1245.9299999999998</v>
+        <v>5119.1419999999998</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -494,6 +497,12 @@
         <f>B4*H3</f>
         <v>586.31999999999994</v>
       </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>7.0039999999999996</v>
+      </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -508,6 +517,21 @@
       <c r="E5">
         <f>B5*H3</f>
         <v>659.61</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>553</v>
+      </c>
+      <c r="C6">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>123</v>
+      </c>
+      <c r="E6">
+        <f>B6*H4</f>
+        <v>3873.2119999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>